<commit_message>
Changes done in spare time: 28-05-2018
</commit_message>
<xml_diff>
--- a/ToolbarOfFunctions/Resources/forTesting2.xlsx
+++ b/ToolbarOfFunctions/Resources/forTesting2.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17985" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="c#" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="VB" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
   <si>
     <t>A</t>
   </si>
@@ -50,18 +50,12 @@
     <t>C:\Temp\sfc\ArchiveFiles.vbs</t>
   </si>
   <si>
-    <t>24/05/2018 20:57:44</t>
-  </si>
-  <si>
     <t>ArchiveFiles.vbs</t>
   </si>
   <si>
     <t>C:\Temp\sfc\ArchiveFiles.vbs.Lnk</t>
   </si>
   <si>
-    <t>24/05/2018 20:57:30</t>
-  </si>
-  <si>
     <t>ArchiveFiles.vbs.Lnk</t>
   </si>
   <si>
@@ -86,18 +80,12 @@
     <t>C:\Temp\sfc\sendEmail.exe</t>
   </si>
   <si>
-    <t>24/05/2018 20:57:31</t>
-  </si>
-  <si>
     <t>sendEmail.exe</t>
   </si>
   <si>
     <t>C:\Temp\sfc\SilentLaunch.exe</t>
   </si>
   <si>
-    <t>24/05/2018 20:57:36</t>
-  </si>
-  <si>
     <t>1.00.0001</t>
   </si>
   <si>
@@ -107,9 +95,6 @@
     <t>C:\Temp\sfc\SpaceSniffer.exe</t>
   </si>
   <si>
-    <t>24/05/2018 20:57:42</t>
-  </si>
-  <si>
     <t>1.3.0.2</t>
   </si>
   <si>
@@ -117,9 +102,6 @@
   </si>
   <si>
     <t>16.21.0.0</t>
-  </si>
-  <si>
-    <t>1.0.0.1</t>
   </si>
   <si>
     <t>File Name</t>
@@ -141,7 +123,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,7 +134,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -178,10 +165,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,144 +577,165 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4">
+        <v>43167.625555555554</v>
+      </c>
+      <c r="C2" s="3">
+        <v>47031</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>47031</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="4">
+        <v>42766.654861111114</v>
+      </c>
+      <c r="C3" s="3">
+        <v>877</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>877</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B4" s="4">
+        <v>43052.495787037034</v>
+      </c>
+      <c r="C4" s="3">
+        <v>62</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1">
-        <v>43081.570428240739</v>
-      </c>
-      <c r="C4">
-        <v>62</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B5" s="4">
+        <v>42856.351365740738</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1458856</v>
+      </c>
+      <c r="D5" s="3">
+        <v>16.21</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>1458856</v>
-      </c>
-      <c r="D5">
-        <v>16.21</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B6" s="4">
+        <v>43046.630925925929</v>
+      </c>
+      <c r="C6" s="3">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1">
-        <v>43081.570428240739</v>
-      </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B7" s="4">
+        <v>37595.877453703702</v>
+      </c>
+      <c r="C7" s="3">
+        <v>454656</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="4">
+        <v>41717.808078703703</v>
+      </c>
+      <c r="C8" s="3">
+        <v>20480</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7">
-        <v>454656</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="4">
+        <v>42645.414618055554</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2309632</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8">
-        <v>20480</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E9" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9">
-        <v>2309632</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -733,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,140 +758,145 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>43167.667222222219</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>47031</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="4">
+        <v>42766.696527777778</v>
+      </c>
+      <c r="C3" s="3">
+        <v>877</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1">
-        <v>42766.696527777778</v>
-      </c>
-      <c r="C3">
-        <v>877</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4">
+        <v>43052.537453703706</v>
+      </c>
+      <c r="C4" s="3">
+        <v>62</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1">
-        <v>43052.537453703706</v>
-      </c>
-      <c r="C4">
-        <v>62</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B5" s="4">
+        <v>42856.351365740738</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1458856</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1">
-        <v>42856.351365740738</v>
-      </c>
-      <c r="C5">
-        <v>1458856</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B6" s="4">
+        <v>43046.672592592593</v>
+      </c>
+      <c r="C6" s="3">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1">
-        <v>43046.672592592593</v>
-      </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B7" s="4">
+        <v>37595.919120370374</v>
+      </c>
+      <c r="C7" s="3">
+        <v>454656</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1">
-        <v>37595.919120370374</v>
-      </c>
-      <c r="C7">
-        <v>454656</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B8" s="4">
+        <v>41717.808078703703</v>
+      </c>
+      <c r="C8" s="3">
+        <v>20480</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1">
-        <v>41717.849745370368</v>
-      </c>
-      <c r="C8">
-        <v>20480</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1">
-        <v>42645.414606481485</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="4">
+        <v>42645.414618055554</v>
+      </c>
+      <c r="C9" s="3">
         <v>2309632</v>
       </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>